<commit_message>
robustness on blank lines
</commit_message>
<xml_diff>
--- a/mass_producer/sheets/生物.xlsx
+++ b/mass_producer/sheets/生物.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifeichen/WorkSpace/GithubRepos/Wizard-s-Deck/mass_producer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifeichen/WorkSpace/GithubRepos/Wizard-s-Deck/mass_producer/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC30DB7-7993-FC46-9A44-95386C17B8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6C6C68-F376-FE4A-8ABC-3B38A17A237D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1860" windowWidth="28040" windowHeight="17260" xr2:uid="{58AF0140-36BA-C749-B66E-B595205C3BA3}"/>
+    <workbookView xWindow="3500" yWindow="5320" windowWidth="28040" windowHeight="17260" xr2:uid="{58AF0140-36BA-C749-B66E-B595205C3BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="火" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>编号</t>
   </si>
@@ -87,13 +87,16 @@
   </si>
   <si>
     <t>牢大，我想你了\n牢大牢大，我想你了牢大，我想你了牢大，我想你了牢大，我想你了牢大，我想你了牢大，我想你了牢大，我想你了</t>
+  </si>
+  <si>
+    <t>风</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,6 +107,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,9 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C332B0-E0A8-D64E-A405-37ABC5A72F50}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,7 +526,38 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>114513</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>